<commit_message>
New backgrounds and blog post updates
</commit_message>
<xml_diff>
--- a/static/publications/Safespring_Kalkyl_LCC.xlsx
+++ b/static/publications/Safespring_Kalkyl_LCC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/safespring/Documents/github/web/static/publications/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE0531FE-04CB-124E-8C54-56CEA3D7BE42}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD08A4F-5F03-1C42-94B5-FE96C4E7877A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{C804E9B0-2B52-E14B-8355-3A1718BC4037}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{C804E9B0-2B52-E14B-8355-3A1718BC4037}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduktion" sheetId="12" r:id="rId1"/>
@@ -3692,7 +3692,9 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1"/>
   <cols>

</xml_diff>